<commit_message>
Add pages report (#11)
</commit_message>
<xml_diff>
--- a/storage/app/exel_templates/full_report.xlsx
+++ b/storage/app/exel_templates/full_report.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\openserver\ospanel\domains\app-main\storage\app\exel_templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="780" windowWidth="27495" windowHeight="11775" activeTab="4"/>
+    <workbookView xWindow="630" yWindow="780" windowWidth="27495" windowHeight="11775"/>
   </bookViews>
   <sheets>
     <sheet name="Статистика по операторам" sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -36,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -194,9 +199,6 @@
     <t>Принято на сумму</t>
   </si>
   <si>
-    <t>[operators]</t>
-  </si>
-  <si>
     <t>[operators.count_lid]</t>
   </si>
   <si>
@@ -227,18 +229,9 @@
     <t>[operators.main_other_sum]</t>
   </si>
   <si>
-    <t>[operator.count_calls]</t>
-  </si>
-  <si>
-    <t>[operator.count_time_calls]</t>
-  </si>
-  <si>
     <t>Длительность звонков(min)</t>
   </si>
   <si>
-    <t>[operator.count_avg_calls]</t>
-  </si>
-  <si>
     <t>[statistic.day.date]</t>
   </si>
   <si>
@@ -345,12 +338,24 @@
   </si>
   <si>
     <t>[resources.confirm_calls]</t>
+  </si>
+  <si>
+    <t>[operators.name]</t>
+  </si>
+  <si>
+    <t>[operators.count_calls]</t>
+  </si>
+  <si>
+    <t>[operators.count_time_calls]</t>
+  </si>
+  <si>
+    <t>[operators.count_avg_calls]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -496,11 +501,11 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -561,7 +566,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,7 +601,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -810,8 +815,8 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -832,10 +837,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -946,7 +951,7 @@
         <v>25</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>26</v>
@@ -957,40 +962,40 @@
     </row>
     <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="17" t="s">
         <v>48</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>49</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>28</v>
@@ -1002,13 +1007,13 @@
         <v>0</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="S5" s="11"/>
     </row>
@@ -1068,8 +1073,8 @@
   </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1086,12 +1091,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1160,41 +1165,41 @@
     </row>
     <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="L4" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="M4" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1256,10 +1261,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1588,7 +1593,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>40</v>
@@ -1610,34 +1615,34 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>28</v>
@@ -1649,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="2"/>
@@ -1722,7 +1727,7 @@
   </sheetPr>
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1740,10 +1745,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1827,40 +1832,40 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="H4" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>

</xml_diff>